<commit_message>
final update, this file is deprecated
</commit_message>
<xml_diff>
--- a/Study.xlsx
+++ b/Study.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Mooc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0B6C7D-73F4-4F08-A640-DB50B208BB36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C05008-EAC2-43B6-B103-4A7D143F4F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12827" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,14 +44,6 @@
     <pivotCache cacheId="0" r:id="rId7"/>
     <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1291,6 +1283,187 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
+      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Microsoft YaHei"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <name val="Microsoft YaHei"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="等线"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="等线"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="176" formatCode="m/d;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="等线"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Microsoft YaHei"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Microsoft YaHei"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Microsoft YaHei"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i/>
@@ -1485,187 +1658,6 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Microsoft YaHei"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <name val="Microsoft YaHei"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="等线"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="等线"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="176" formatCode="m/d;@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="等线"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Microsoft YaHei"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Microsoft YaHei"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Microsoft YaHei"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -16469,10 +16461,10 @@
     <dataField name="求和项:duration(hrs)" fld="4" baseField="0" baseItem="0" numFmtId="180"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="19">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -17314,10 +17306,10 @@
     <dataField name="求和项:duration(hrs)" fld="4" baseField="0" baseItem="0" numFmtId="180"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="17">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -17345,19 +17337,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="项目" displayName="项目" ref="B2:H11" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="项目" displayName="项目" ref="B2:H11" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="course" totalsRowLabel="Total" dataDxfId="26" dataCellStyle="Indent"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="due" dataDxfId="25" dataCellStyle="Indent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="course" totalsRowLabel="Total" dataDxfId="10" dataCellStyle="Indent"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="due" dataDxfId="9" dataCellStyle="Indent">
       <calculatedColumnFormula>项目[[#This Row],[next]] - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="next" dataDxfId="24" dataCellStyle="Indent"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="finish" dataDxfId="23" dataCellStyle="Indent"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="all" dataDxfId="22" dataCellStyle="Indent"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="progress" totalsRowFunction="count" dataDxfId="21">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="next" dataDxfId="8" dataCellStyle="Indent"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="finish" dataDxfId="7" dataCellStyle="Indent"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="all" dataDxfId="6" dataCellStyle="Indent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="progress" totalsRowFunction="count" dataDxfId="5">
       <calculatedColumnFormula>项目[[#This Row],[finish]]/项目[[#This Row],[all]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="link" totalsRowFunction="count" dataDxfId="20" dataCellStyle="超链接"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="link" totalsRowFunction="count" dataDxfId="4" dataCellStyle="超链接"/>
   </tableColumns>
   <tableStyleInfo name="Weekly Planner Tables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -17657,7 +17649,7 @@
       </c>
       <c r="C3" s="47">
         <f ca="1">项目[[#This Row],[next]] - TODAY()</f>
-        <v>-43863</v>
+        <v>-44268</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="9">
@@ -17685,7 +17677,7 @@
       </c>
       <c r="C4" s="47">
         <f ca="1">项目[[#This Row],[next]] - TODAY()</f>
-        <v>-43863</v>
+        <v>-44268</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="9">
@@ -17713,7 +17705,7 @@
       </c>
       <c r="C5" s="47">
         <f ca="1">项目[[#This Row],[next]] - TODAY()</f>
-        <v>-43863</v>
+        <v>-44268</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="9">
@@ -17921,34 +17913,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="15" priority="102" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="102" operator="lessThan">
       <formula>1.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="104" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="104" operator="between">
       <formula>7</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="105" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="105" operator="between">
       <formula>14</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="106" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="11" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="79" operator="lessThan">
       <formula>1.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="80" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="80" operator="between">
       <formula>7</formula>
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="81" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="81" operator="between">
       <formula>14</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="82" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17967,34 +17959,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="lessThan">
       <formula>1.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="between">
       <formula>7</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="between">
       <formula>14</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
       <formula>1.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
       <formula>7</formula>
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="between">
       <formula>14</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20743,7 +20735,7 @@
   </sheetPr>
   <dimension ref="A1:BD270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -52435,143 +52427,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <APDescription xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AssetExpire xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">2029-01-01T08:00:00+00:00</AssetExpire>
-    <CampaignTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </CampaignTagsTaxHTField0>
-    <IntlLangReviewDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TPFriendlyName xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <IntlLangReview xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IntlLangReview>
-    <LocLastLocAttemptVersionLookup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">845893</LocLastLocAttemptVersionLookup>
-    <PolicheckWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <SubmitterId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AcquiredFrom xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Internal MS</AcquiredFrom>
-    <EditorialStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <Markets xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
-    <OriginAsset xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AssetStart xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">2012-06-28T22:29:33+00:00</AssetStart>
-    <FriendlyTitle xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <MarketSpecific xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</MarketSpecific>
-    <TPNamespace xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <PublishStatusLookup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Value>477958</Value>
-    </PublishStatusLookup>
-    <APAuthor xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId>2566</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </APAuthor>
-    <TPCommandLine xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <IntlLangReviewer xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <OpenTemplate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">true</OpenTemplate>
-    <CSXSubmissionDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TaxCatchAll xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
-    <Manager xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <NumericId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <ParentAssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <OriginalSourceMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">english</OriginalSourceMarket>
-    <ApprovalStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">InProgress</ApprovalStatus>
-    <TPComponent xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <EditorialTags xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TPExecutable xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TPLaunchHelpLink xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <LocComments xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <LocRecommendedHandoff xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <SourceTitle xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <CSXUpdate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</CSXUpdate>
-    <IntlLocPriority xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <UAProjectedTotalWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AssetType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <MachineTranslated xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</MachineTranslated>
-    <OutputCachingOn xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</OutputCachingOn>
-    <TemplateStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Complete</TemplateStatus>
-    <IsSearchable xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IsSearchable>
-    <ContentItem xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <HandoffToMSDN xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <ShowIn xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Show everywhere</ShowIn>
-    <ThumbnailAssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <UALocComments xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <UALocRecommendation xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Localize</UALocRecommendation>
-    <LastModifiedDateTime xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <LegacyData xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <LocManualTestRequired xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</LocManualTestRequired>
-    <LocMarketGroupTiers2 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <ClipArtFilename xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TPApplication xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <CSXHash xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <DirectSourceMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">english</DirectSourceMarket>
-    <PrimaryImageGen xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</PrimaryImageGen>
-    <PlannedPubDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <CSXSubmissionMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <Downloads xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">0</Downloads>
-    <ArtSampleDocs xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TrustLevel xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">1 Microsoft Managed Content</TrustLevel>
-    <BlockPublish xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</BlockPublish>
-    <TPLaunchHelpLinkType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Template</TPLaunchHelpLinkType>
-    <LocalizationTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </LocalizationTagsTaxHTField0>
-    <BusinessGroup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <Providers xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TemplateTemplateType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Excel Spreadsheet Template</TemplateTemplateType>
-    <TimesCloned xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <TPAppVersion xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <VoteCount xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AverageRating xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <FeatureTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </FeatureTagsTaxHTField0>
-    <Provider xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <UACurrentWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <AssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">TP102929987</AssetId>
-    <TPClientViewer xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <DSATActionTaken xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <APEditor xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </APEditor>
-    <TPInstallLocation xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <OOCacheId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <IsDeleted xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IsDeleted>
-    <PublishTargets xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">OfficeOnlineVNext</PublishTargets>
-    <ApprovalLog xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <BugNumber xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <CrawlForDependencies xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</CrawlForDependencies>
-    <InternalTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </InternalTagsTaxHTField0>
-    <LastHandOff xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <Milestone xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <OriginalRelease xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">15</OriginalRelease>
-    <RecommendationsModifier xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <ScenarioTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ScenarioTagsTaxHTField0>
-    <UANotes xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
-    <Description0 xmlns="a0b64b53-fba7-43ca-b952-90e5e74773dd" xsi:nil="true"/>
-    <Component0 xmlns="a0b64b53-fba7-43ca-b952-90e5e74773dd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x0101008D8B3457135D67479991424C624CBB4704002439B9162B2E88498A324BEFF3815221" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7e4f43ee53fc86ae1dd6272262eb9fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="905c3888-6285-45d0-bd76-60a9ac2d738c" xmlns:ns3="a0b64b53-fba7-43ca-b952-90e5e74773dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12cd52f9b34cd953802493d919c383c5" ns2:_="" ns3:_="">
     <xsd:import namespace="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
@@ -53630,10 +53485,158 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <APDescription xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AssetExpire xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">2029-01-01T08:00:00+00:00</AssetExpire>
+    <CampaignTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </CampaignTagsTaxHTField0>
+    <IntlLangReviewDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TPFriendlyName xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <IntlLangReview xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IntlLangReview>
+    <LocLastLocAttemptVersionLookup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">845893</LocLastLocAttemptVersionLookup>
+    <PolicheckWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <SubmitterId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AcquiredFrom xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Internal MS</AcquiredFrom>
+    <EditorialStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <Markets xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
+    <OriginAsset xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AssetStart xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">2012-06-28T22:29:33+00:00</AssetStart>
+    <FriendlyTitle xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <MarketSpecific xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</MarketSpecific>
+    <TPNamespace xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <PublishStatusLookup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Value>477958</Value>
+    </PublishStatusLookup>
+    <APAuthor xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId>2566</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </APAuthor>
+    <TPCommandLine xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <IntlLangReviewer xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <OpenTemplate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">true</OpenTemplate>
+    <CSXSubmissionDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TaxCatchAll xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
+    <Manager xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <NumericId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <ParentAssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <OriginalSourceMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">english</OriginalSourceMarket>
+    <ApprovalStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">InProgress</ApprovalStatus>
+    <TPComponent xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <EditorialTags xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TPExecutable xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TPLaunchHelpLink xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <LocComments xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <LocRecommendedHandoff xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <SourceTitle xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <CSXUpdate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</CSXUpdate>
+    <IntlLocPriority xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <UAProjectedTotalWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AssetType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <MachineTranslated xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</MachineTranslated>
+    <OutputCachingOn xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</OutputCachingOn>
+    <TemplateStatus xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Complete</TemplateStatus>
+    <IsSearchable xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IsSearchable>
+    <ContentItem xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <HandoffToMSDN xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <ShowIn xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Show everywhere</ShowIn>
+    <ThumbnailAssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <UALocComments xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <UALocRecommendation xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Localize</UALocRecommendation>
+    <LastModifiedDateTime xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <LegacyData xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <LocManualTestRequired xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</LocManualTestRequired>
+    <LocMarketGroupTiers2 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <ClipArtFilename xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TPApplication xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <CSXHash xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <DirectSourceMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">english</DirectSourceMarket>
+    <PrimaryImageGen xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</PrimaryImageGen>
+    <PlannedPubDate xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <CSXSubmissionMarket xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <Downloads xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">0</Downloads>
+    <ArtSampleDocs xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TrustLevel xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">1 Microsoft Managed Content</TrustLevel>
+    <BlockPublish xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</BlockPublish>
+    <TPLaunchHelpLinkType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Template</TPLaunchHelpLinkType>
+    <LocalizationTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </LocalizationTagsTaxHTField0>
+    <BusinessGroup xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <Providers xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TemplateTemplateType xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">Excel Spreadsheet Template</TemplateTemplateType>
+    <TimesCloned xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <TPAppVersion xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <VoteCount xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AverageRating xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <FeatureTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </FeatureTagsTaxHTField0>
+    <Provider xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <UACurrentWords xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <AssetId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">TP102929987</AssetId>
+    <TPClientViewer xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <DSATActionTaken xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <APEditor xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </APEditor>
+    <TPInstallLocation xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <OOCacheId xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <IsDeleted xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</IsDeleted>
+    <PublishTargets xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">OfficeOnlineVNext</PublishTargets>
+    <ApprovalLog xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <BugNumber xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <CrawlForDependencies xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">false</CrawlForDependencies>
+    <InternalTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </InternalTagsTaxHTField0>
+    <LastHandOff xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <Milestone xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <OriginalRelease xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">15</OriginalRelease>
+    <RecommendationsModifier xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <ScenarioTagsTaxHTField0 xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ScenarioTagsTaxHTField0>
+    <UANotes xmlns="905c3888-6285-45d0-bd76-60a9ac2d738c" xsi:nil="true"/>
+    <Description0 xmlns="a0b64b53-fba7-43ca-b952-90e5e74773dd" xsi:nil="true"/>
+    <Component0 xmlns="a0b64b53-fba7-43ca-b952-90e5e74773dd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEE221-42CE-4499-AA86-34AC294DC780}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E974EB3C-D0ED-4B3B-9891-37E7C0804F16}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
+    <ds:schemaRef ds:uri="a0b64b53-fba7-43ca-b952-90e5e74773dd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -53656,20 +53659,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E974EB3C-D0ED-4B3B-9891-37E7C0804F16}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEE221-42CE-4499-AA86-34AC294DC780}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="905c3888-6285-45d0-bd76-60a9ac2d738c"/>
-    <ds:schemaRef ds:uri="a0b64b53-fba7-43ca-b952-90e5e74773dd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>